<commit_message>
Updates to the documentation and addition of the template for the Broad single-cell portal (SCP) following the Alexandria convention
</commit_message>
<xml_diff>
--- a/Templates/GEO-templates/MIATE_GEOSubmissionFields_SCP-AlexandriaFormat.xlsx
+++ b/Templates/GEO-templates/MIATE_GEOSubmissionFields_SCP-AlexandriaFormat.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/MIATE/Templates/GEO-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:40009_{4B9E2D4B-C2D4-436A-80BB-680C3B1E2178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE8F4A9B-D8BE-4F84-B20A-21DC0FE05E09}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:40009_{4B9E2D4B-C2D4-436A-80BB-680C3B1E2178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D1E12DD-63E8-4241-8BC6-FF8C9AE02271}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prj168_Statin_TCDD-metadata" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="140">
   <si>
     <t>species</t>
   </si>
@@ -437,6 +438,9 @@
   </si>
   <si>
     <t>ALPHA-dri (Shepherd Specialty Papers)</t>
+  </si>
+  <si>
+    <t>DSSToxID</t>
   </si>
 </sst>
 </file>
@@ -1310,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BM13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,7 +1498,9 @@
       <c r="AK1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="1"/>
+      <c r="AL1" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="AM1" s="1" t="s">
         <v>34</v>
       </c>
@@ -3921,4 +3927,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90D42C7-ABA7-4016-A71E-19A39DD24B43}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>